<commit_message>
starting to understand IRMs/MaxPointsReason codes in Barbados result format
</commit_message>
<xml_diff>
--- a/java/com.sap.sailing.barbados.resultimport.test/resources/RESULTS-505Barbados.xlsx
+++ b/java/com.sap.sailing.barbados.resultimport.test/resources/RESULTS-505Barbados.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="13425" windowHeight="7485" tabRatio="778" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="13425" windowHeight="7485" tabRatio="778" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="INSTRUCTIONS FOR USE" sheetId="33" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2829" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2831" uniqueCount="246">
   <si>
     <t>GER</t>
   </si>
@@ -1232,6 +1232,12 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1239,12 +1245,6 @@
     </xf>
     <xf numFmtId="15" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -1611,15 +1611,15 @@
       <c r="I7" s="62"/>
     </row>
     <row r="8" spans="1:9" ht="15.95" customHeight="1">
-      <c r="A8" s="66"/>
-      <c r="B8" s="66"/>
-      <c r="C8" s="66"/>
-      <c r="D8" s="66"/>
-      <c r="E8" s="66"/>
-      <c r="F8" s="66"/>
-      <c r="G8" s="66"/>
-      <c r="H8" s="66"/>
-      <c r="I8" s="66"/>
+      <c r="A8" s="63"/>
+      <c r="B8" s="63"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="63"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="63"/>
+      <c r="G8" s="63"/>
+      <c r="H8" s="63"/>
+      <c r="I8" s="63"/>
     </row>
     <row r="9" spans="1:9" ht="19.5" customHeight="1">
       <c r="A9" s="62" t="s">
@@ -1653,31 +1653,31 @@
       <c r="A11" s="54">
         <v>2</v>
       </c>
-      <c r="B11" s="67" t="s">
+      <c r="B11" s="64" t="s">
         <v>232</v>
       </c>
-      <c r="C11" s="67"/>
-      <c r="D11" s="67"/>
-      <c r="E11" s="67"/>
-      <c r="F11" s="67"/>
-      <c r="G11" s="67"/>
-      <c r="H11" s="67"/>
-      <c r="I11" s="67"/>
+      <c r="C11" s="64"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="64"/>
+      <c r="H11" s="64"/>
+      <c r="I11" s="64"/>
     </row>
     <row r="12" spans="1:9" s="55" customFormat="1" ht="31.5" customHeight="1">
       <c r="A12" s="54">
         <v>3</v>
       </c>
-      <c r="B12" s="67" t="s">
+      <c r="B12" s="64" t="s">
         <v>235</v>
       </c>
-      <c r="C12" s="67"/>
-      <c r="D12" s="67"/>
-      <c r="E12" s="67"/>
-      <c r="F12" s="67"/>
-      <c r="G12" s="67"/>
-      <c r="H12" s="67"/>
-      <c r="I12" s="67"/>
+      <c r="C12" s="64"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="64"/>
+      <c r="F12" s="64"/>
+      <c r="G12" s="64"/>
+      <c r="H12" s="64"/>
+      <c r="I12" s="64"/>
     </row>
     <row r="13" spans="1:9" s="55" customFormat="1" ht="47.25" customHeight="1">
       <c r="A13" s="54">
@@ -1713,29 +1713,29 @@
       <c r="A15" s="54">
         <v>6</v>
       </c>
-      <c r="B15" s="63" t="s">
+      <c r="B15" s="65" t="s">
         <v>236</v>
       </c>
-      <c r="C15" s="63"/>
-      <c r="D15" s="63"/>
-      <c r="E15" s="63"/>
-      <c r="F15" s="63"/>
-      <c r="G15" s="63"/>
-      <c r="H15" s="63"/>
-      <c r="I15" s="63"/>
+      <c r="C15" s="65"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="65"/>
+      <c r="F15" s="65"/>
+      <c r="G15" s="65"/>
+      <c r="H15" s="65"/>
+      <c r="I15" s="65"/>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="64" t="s">
+      <c r="A17" s="66" t="s">
         <v>238</v>
       </c>
-      <c r="B17" s="64"/>
-      <c r="C17" s="64"/>
-      <c r="D17" s="64"/>
-      <c r="E17" s="64"/>
-      <c r="F17" s="64"/>
-      <c r="G17" s="64"/>
-      <c r="H17" s="64"/>
-      <c r="I17" s="64"/>
+      <c r="B17" s="66"/>
+      <c r="C17" s="66"/>
+      <c r="D17" s="66"/>
+      <c r="E17" s="66"/>
+      <c r="F17" s="66"/>
+      <c r="G17" s="66"/>
+      <c r="H17" s="66"/>
+      <c r="I17" s="66"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="53" t="s">
@@ -1743,24 +1743,24 @@
       </c>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="65">
+      <c r="A20" s="67">
         <v>41371</v>
       </c>
-      <c r="B20" s="65"/>
+      <c r="B20" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B13:I13"/>
+    <mergeCell ref="B14:I14"/>
+    <mergeCell ref="B15:I15"/>
+    <mergeCell ref="A17:I17"/>
+    <mergeCell ref="A20:B20"/>
     <mergeCell ref="A7:I7"/>
     <mergeCell ref="A8:I8"/>
     <mergeCell ref="A9:I9"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="B12:I12"/>
     <mergeCell ref="B10:I10"/>
-    <mergeCell ref="B13:I13"/>
-    <mergeCell ref="B14:I14"/>
-    <mergeCell ref="B15:I15"/>
-    <mergeCell ref="A17:I17"/>
-    <mergeCell ref="A20:B20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1772,7 +1772,7 @@
   <dimension ref="A1:G81"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="18" customHeight="1"/>
@@ -1818,10 +1818,12 @@
       <c r="D2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="10"/>
+      <c r="E2" s="10">
+        <v>7</v>
+      </c>
       <c r="G2" s="12">
         <f>E2</f>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1">
@@ -1837,10 +1839,12 @@
       <c r="D3" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="10"/>
+      <c r="E3" s="10">
+        <v>9</v>
+      </c>
       <c r="G3" s="12">
         <f t="shared" ref="G3:G66" si="0">E3</f>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="18" customHeight="1">
@@ -1856,10 +1860,12 @@
       <c r="D4" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="10"/>
+      <c r="E4" s="10">
+        <v>7</v>
+      </c>
       <c r="G4" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="18" customHeight="1">
@@ -3281,8 +3287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G82"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="18" customHeight="1"/>
@@ -3328,10 +3334,12 @@
       <c r="D2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="10"/>
+      <c r="E2" s="10">
+        <v>3</v>
+      </c>
       <c r="G2" s="12">
         <f>E2</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1">
@@ -3347,10 +3355,12 @@
       <c r="D3" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="10"/>
+      <c r="E3" s="10">
+        <v>2</v>
+      </c>
       <c r="G3" s="12">
         <f t="shared" ref="G3:G7" si="0">E3</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="18" customHeight="1">
@@ -3366,10 +3376,12 @@
       <c r="D4" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="10"/>
+      <c r="E4" s="10">
+        <v>5</v>
+      </c>
       <c r="G4" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="18" customHeight="1">
@@ -7872,7 +7884,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AL101"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="D1" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="D1" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AI2" sqref="AI2"/>
     </sheetView>
@@ -8015,15 +8027,15 @@
       </c>
       <c r="F2" s="7">
         <f>VLOOKUP(C2,'RACE-1'!$B$2:$E$91,4,FALSE)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G2" s="4">
         <f>VLOOKUP(C2,'RACE-2'!$B$2:$E$100,4,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="H2" s="4">
+        <v>7</v>
+      </c>
+      <c r="H2" s="4" t="str">
         <f>VLOOKUP(C2,'RACE-3'!$B$2:$E$100,4,FALSE)</f>
-        <v>0</v>
+        <v>DNF</v>
       </c>
       <c r="I2" s="4">
         <f>VLOOKUP(C2,'RACE-4'!$B$2:$E$100,4,FALSE)</f>
@@ -8051,23 +8063,23 @@
       </c>
       <c r="O2" s="4">
         <f>SUM(F2:N2)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="P2" s="4">
         <f>IF(AI2&lt;4,AC2, IF(3&lt;AI2&lt;8,AD2, IF(AI2&gt;7,AE2)))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="R2" s="4">
         <f>VLOOKUP(C2,'RACE-1'!$B$2:$G$100,6,FALSE)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S2" s="4">
         <f>VLOOKUP(C2,'RACE-2'!$B$2:$G$100,6,FALSE)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="T2" s="4">
         <f>VLOOKUP(C2,'RACE-3'!$B$2:$G$100,6,FALSE)</f>
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="U2" s="4">
         <f>VLOOKUP(C2,'RACE-4'!$B$2:$G$100,6,FALSE)</f>
@@ -8095,31 +8107,31 @@
       </c>
       <c r="AB2" s="4">
         <f>SUM(R2:Z2)</f>
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="AC2" s="5">
         <f>O2</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AD2" s="5">
         <f>AB2-AG2</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AE2" s="5">
         <f>AB2-(AG2+AH2)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AG2" s="5">
         <f>LARGE(R2:Z2,1)</f>
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="AH2" s="5">
         <f>LARGE(R2:Z2,2)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AI2" s="22">
         <f>COUNTIF(R2:Z2,"&gt;0")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:35" ht="20.100000000000001" customHeight="1">
@@ -8137,15 +8149,15 @@
       </c>
       <c r="F3" s="7">
         <f>VLOOKUP(C3,'RACE-1'!$B$2:$E$91,4,FALSE)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G3" s="4">
         <f>VLOOKUP(C3,'RACE-2'!$B$2:$E$100,4,FALSE)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H3" s="4">
         <f>VLOOKUP(C3,'RACE-3'!$B$2:$E$100,4,FALSE)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="I3" s="4">
         <f>VLOOKUP(C3,'RACE-4'!$B$2:$E$100,4,FALSE)</f>
@@ -8173,23 +8185,23 @@
       </c>
       <c r="O3" s="4">
         <f t="shared" ref="O3:O10" si="0">SUM(F3:N3)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="P3" s="4">
         <f t="shared" ref="P3:P66" si="1">IF(AI3&lt;4,AC3, IF(3&lt;AI3&lt;8,AD3, IF(AI3&gt;7,AE3)))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="R3" s="4">
         <f>VLOOKUP(C3,'RACE-1'!$B$2:$G$100,6,FALSE)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S3" s="4">
         <f>VLOOKUP(C3,'RACE-2'!$B$2:$G$100,6,FALSE)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="T3" s="4">
         <f>VLOOKUP(C3,'RACE-3'!$B$2:$G$100,6,FALSE)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="U3" s="4">
         <f>VLOOKUP(C3,'RACE-4'!$B$2:$G$100,6,FALSE)</f>
@@ -8217,31 +8229,31 @@
       </c>
       <c r="AB3" s="4">
         <f t="shared" ref="AB3:AB10" si="2">SUM(R3:Z3)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AC3" s="5">
         <f t="shared" ref="AC3:AC10" si="3">O3</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AD3" s="5">
         <f t="shared" ref="AD3:AD10" si="4">AB3-AG3</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="AE3" s="5">
         <f t="shared" ref="AE3:AE10" si="5">AB3-(AG3+AH3)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AG3" s="5">
         <f t="shared" ref="AG3:AG66" si="6">LARGE(R3:Z3,1)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AH3" s="5">
         <f t="shared" ref="AH3:AH66" si="7">LARGE(R3:Z3,2)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AI3" s="22">
         <f t="shared" ref="AI3:AI66" si="8">COUNTIF(R3:Z3,"&gt;0")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:35" ht="20.100000000000001" customHeight="1">
@@ -8259,15 +8271,15 @@
       </c>
       <c r="F4" s="7">
         <f>VLOOKUP(C4,'RACE-1'!$B$2:$E$91,4,FALSE)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G4" s="4">
         <f>VLOOKUP(C4,'RACE-2'!$B$2:$E$100,4,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="H4" s="4">
+        <v>7</v>
+      </c>
+      <c r="H4" s="4" t="str">
         <f>VLOOKUP(C4,'RACE-3'!$B$2:$E$100,4,FALSE)</f>
-        <v>0</v>
+        <v>OCS</v>
       </c>
       <c r="I4" s="4">
         <f>VLOOKUP(C4,'RACE-4'!$B$2:$E$100,4,FALSE)</f>
@@ -8295,23 +8307,23 @@
       </c>
       <c r="O4" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="P4" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="R4" s="4">
         <f>VLOOKUP(C4,'RACE-1'!$B$2:$G$100,6,FALSE)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="S4" s="4">
         <f>VLOOKUP(C4,'RACE-2'!$B$2:$G$100,6,FALSE)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="T4" s="4">
         <f>VLOOKUP(C4,'RACE-3'!$B$2:$G$100,6,FALSE)</f>
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="U4" s="4">
         <f>VLOOKUP(C4,'RACE-4'!$B$2:$G$100,6,FALSE)</f>
@@ -8339,31 +8351,31 @@
       </c>
       <c r="AB4" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="AC4" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AD4" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AE4" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AG4" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="AH4" s="5">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AI4" s="22">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:35" ht="20.100000000000001" customHeight="1">
@@ -28984,8 +28996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G82"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A31" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41:E42"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="18" customHeight="1"/>
@@ -29031,10 +29043,11 @@
       <c r="D2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="10"/>
+      <c r="E2" s="10" t="s">
+        <v>177</v>
+      </c>
       <c r="G2" s="12">
-        <f>E2</f>
-        <v>0</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1">
@@ -29050,10 +29063,12 @@
       <c r="D3" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="10"/>
+      <c r="E3" s="10">
+        <v>9</v>
+      </c>
       <c r="G3" s="12">
         <f t="shared" ref="G3:G66" si="0">E3</f>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="18" customHeight="1">
@@ -29069,10 +29084,11 @@
       <c r="D4" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="10"/>
+      <c r="E4" s="10" t="s">
+        <v>172</v>
+      </c>
       <c r="G4" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="18" customHeight="1">

</xml_diff>

<commit_message>
the result format for Barbados changed a column header; adjusted importer and tests
</commit_message>
<xml_diff>
--- a/java/com.sap.sailing.barbados.resultimport.test/resources/RESULTS-505Barbados.xlsx
+++ b/java/com.sap.sailing.barbados.resultimport.test/resources/RESULTS-505Barbados.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="13425" windowHeight="7485" tabRatio="778" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="17085" windowHeight="4305" tabRatio="778" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="INSTRUCTIONS FOR USE" sheetId="33" r:id="rId1"/>
@@ -35,11 +35,12 @@
     <definedName name="_xlnm.Print_Area" localSheetId="2">'RACE-9'!$A$1:$E$81</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
+  <oleSize ref="D1:V9"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2831" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2831" uniqueCount="245">
   <si>
     <t>GER</t>
   </si>
@@ -719,9 +720,6 @@
     <t>RACE 9</t>
   </si>
   <si>
-    <t>RACE SCORE</t>
-  </si>
-  <si>
     <t>SAP 5O5 WORLD CHAMPIONSHIP, BARBADOS, 2013</t>
   </si>
   <si>
@@ -1232,12 +1230,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1245,6 +1237,12 @@
     </xf>
     <xf numFmtId="15" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -1583,23 +1581,23 @@
   <sheetData>
     <row r="2" spans="1:9" s="36" customFormat="1">
       <c r="A2" s="36" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="36" customFormat="1"/>
     <row r="4" spans="1:9" s="36" customFormat="1">
       <c r="A4" s="36" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="36" customFormat="1">
       <c r="A5" s="36" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="66.75" customHeight="1">
       <c r="A7" s="62" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B7" s="62"/>
       <c r="C7" s="62"/>
@@ -1611,19 +1609,19 @@
       <c r="I7" s="62"/>
     </row>
     <row r="8" spans="1:9" ht="15.95" customHeight="1">
-      <c r="A8" s="63"/>
-      <c r="B8" s="63"/>
-      <c r="C8" s="63"/>
-      <c r="D8" s="63"/>
-      <c r="E8" s="63"/>
-      <c r="F8" s="63"/>
-      <c r="G8" s="63"/>
-      <c r="H8" s="63"/>
-      <c r="I8" s="63"/>
+      <c r="A8" s="66"/>
+      <c r="B8" s="66"/>
+      <c r="C8" s="66"/>
+      <c r="D8" s="66"/>
+      <c r="E8" s="66"/>
+      <c r="F8" s="66"/>
+      <c r="G8" s="66"/>
+      <c r="H8" s="66"/>
+      <c r="I8" s="66"/>
     </row>
     <row r="9" spans="1:9" ht="19.5" customHeight="1">
       <c r="A9" s="62" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B9" s="62"/>
       <c r="C9" s="62"/>
@@ -1639,7 +1637,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="62" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C10" s="62"/>
       <c r="D10" s="62"/>
@@ -1653,38 +1651,38 @@
       <c r="A11" s="54">
         <v>2</v>
       </c>
-      <c r="B11" s="64" t="s">
-        <v>232</v>
-      </c>
-      <c r="C11" s="64"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="64"/>
-      <c r="G11" s="64"/>
-      <c r="H11" s="64"/>
-      <c r="I11" s="64"/>
+      <c r="B11" s="67" t="s">
+        <v>231</v>
+      </c>
+      <c r="C11" s="67"/>
+      <c r="D11" s="67"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="67"/>
+      <c r="G11" s="67"/>
+      <c r="H11" s="67"/>
+      <c r="I11" s="67"/>
     </row>
     <row r="12" spans="1:9" s="55" customFormat="1" ht="31.5" customHeight="1">
       <c r="A12" s="54">
         <v>3</v>
       </c>
-      <c r="B12" s="64" t="s">
-        <v>235</v>
-      </c>
-      <c r="C12" s="64"/>
-      <c r="D12" s="64"/>
-      <c r="E12" s="64"/>
-      <c r="F12" s="64"/>
-      <c r="G12" s="64"/>
-      <c r="H12" s="64"/>
-      <c r="I12" s="64"/>
+      <c r="B12" s="67" t="s">
+        <v>234</v>
+      </c>
+      <c r="C12" s="67"/>
+      <c r="D12" s="67"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="67"/>
+      <c r="H12" s="67"/>
+      <c r="I12" s="67"/>
     </row>
     <row r="13" spans="1:9" s="55" customFormat="1" ht="47.25" customHeight="1">
       <c r="A13" s="54">
         <v>4</v>
       </c>
       <c r="B13" s="62" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C13" s="62"/>
       <c r="D13" s="62"/>
@@ -1699,7 +1697,7 @@
         <v>5</v>
       </c>
       <c r="B14" s="62" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C14" s="62"/>
       <c r="D14" s="62"/>
@@ -1713,54 +1711,54 @@
       <c r="A15" s="54">
         <v>6</v>
       </c>
-      <c r="B15" s="65" t="s">
-        <v>236</v>
-      </c>
-      <c r="C15" s="65"/>
-      <c r="D15" s="65"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="65"/>
-      <c r="G15" s="65"/>
-      <c r="H15" s="65"/>
-      <c r="I15" s="65"/>
+      <c r="B15" s="63" t="s">
+        <v>235</v>
+      </c>
+      <c r="C15" s="63"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="63"/>
+      <c r="H15" s="63"/>
+      <c r="I15" s="63"/>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="66" t="s">
-        <v>238</v>
-      </c>
-      <c r="B17" s="66"/>
-      <c r="C17" s="66"/>
-      <c r="D17" s="66"/>
-      <c r="E17" s="66"/>
-      <c r="F17" s="66"/>
-      <c r="G17" s="66"/>
-      <c r="H17" s="66"/>
-      <c r="I17" s="66"/>
+      <c r="A17" s="64" t="s">
+        <v>237</v>
+      </c>
+      <c r="B17" s="64"/>
+      <c r="C17" s="64"/>
+      <c r="D17" s="64"/>
+      <c r="E17" s="64"/>
+      <c r="F17" s="64"/>
+      <c r="G17" s="64"/>
+      <c r="H17" s="64"/>
+      <c r="I17" s="64"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="53" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="67">
+      <c r="A20" s="65">
         <v>41371</v>
       </c>
-      <c r="B20" s="67"/>
+      <c r="B20" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B13:I13"/>
-    <mergeCell ref="B14:I14"/>
-    <mergeCell ref="B15:I15"/>
-    <mergeCell ref="A17:I17"/>
-    <mergeCell ref="A20:B20"/>
     <mergeCell ref="A7:I7"/>
     <mergeCell ref="A8:I8"/>
     <mergeCell ref="A9:I9"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="B12:I12"/>
     <mergeCell ref="B10:I10"/>
+    <mergeCell ref="B13:I13"/>
+    <mergeCell ref="B14:I14"/>
+    <mergeCell ref="B15:I15"/>
+    <mergeCell ref="A17:I17"/>
+    <mergeCell ref="A20:B20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4983,7 +4981,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:F82"/>
+  <dimension ref="A1:G82"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
@@ -5002,7 +5000,7 @@
   <sheetData>
     <row r="1" spans="2:6">
       <c r="B1" s="68" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C1" s="69"/>
       <c r="D1" s="69"/>
@@ -5012,7 +5010,7 @@
     <row r="2" spans="2:6">
       <c r="B2" s="42"/>
       <c r="C2" s="68" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D2" s="69"/>
       <c r="E2" s="69"/>
@@ -5020,7 +5018,7 @@
     </row>
     <row r="3" spans="2:6">
       <c r="B3" s="68" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C3" s="69"/>
       <c r="D3" s="69"/>
@@ -5033,7 +5031,7 @@
       <c r="D4" s="57"/>
       <c r="E4" s="57"/>
       <c r="F4" s="58" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5" spans="2:6" s="59" customFormat="1" ht="51">
@@ -5042,13 +5040,13 @@
       </c>
       <c r="C5" s="60"/>
       <c r="D5" s="61" t="s">
+        <v>243</v>
+      </c>
+      <c r="E5" s="61" t="s">
+        <v>243</v>
+      </c>
+      <c r="F5" s="59" t="s">
         <v>244</v>
-      </c>
-      <c r="E5" s="61" t="s">
-        <v>244</v>
-      </c>
-      <c r="F5" s="59" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="14.25">
@@ -7884,9 +7882,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AL101"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="D1" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="D1" zoomScale="90" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AI2" sqref="AI2"/>
+      <selection pane="bottomLeft" activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -7952,7 +7950,7 @@
         <v>225</v>
       </c>
       <c r="O1" s="52" t="s">
-        <v>226</v>
+        <v>210</v>
       </c>
       <c r="P1" s="52" t="s">
         <v>10</v>
@@ -27486,7 +27484,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G81"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageLayout" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
@@ -28996,7 +28994,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G82"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>

</xml_diff>